<commit_message>
Verif de code 1D
</commit_message>
<xml_diff>
--- a/data/Verif_Code.xlsx
+++ b/data/Verif_Code.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a2d04f23f7faf3ef/Bureau/PROFESSIONAL/CANADA/5_Cours/H25_MEC8211/0_Devoir 1/MEC8211_projet/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{C5DE95D0-53A6-4465-ADD7-FC96FAD8553C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A2898D3-981A-41BB-B7B8-656C2DD7B3B7}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{C5DE95D0-53A6-4465-ADD7-FC96FAD8553C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF3B04D1-51B5-4A5A-BAC5-54B7F7BD1702}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{5642C43C-961F-4D27-AFBA-005B79154A3A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Dx</t>
   </si>
@@ -114,12 +114,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +588,7 @@
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-GB"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -812,7 +811,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-GB"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -934,7 +933,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-GB"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2186,16 +2185,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>706437</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>134540</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>416718</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>170258</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>587375</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>139303</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>551656</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>175021</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2542,8 +2541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F63344-A5D2-4AE2-AC45-BD1F35E35E11}">
   <dimension ref="B1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2600,7 +2599,7 @@
       <c r="C3" s="2">
         <v>1.6074999999999999E-2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <f>($H$5*$H$4^3)/(3*$J$3*$H$2)</f>
         <v>4.7999625002929669</v>
       </c>
@@ -2667,7 +2666,7 @@
         <v>1.6087000000000001E-2</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D3:D8" si="2">($H$5*$H$4^3)/(3*$J$3*$H$2)</f>
+        <f t="shared" ref="D5:D8" si="2">($H$5*$H$4^3)/(3*$J$3*$H$2)</f>
         <v>4.7999625002929669</v>
       </c>
       <c r="E5" s="3">
@@ -2758,6 +2757,9 @@
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
       <c r="E16" t="s">
         <v>11</v>
       </c>
@@ -2793,7 +2795,7 @@
         <v>4.7702999999999998</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D17:D21" si="3">($H$5*$H$4^3)/(3*$J$3*$H$2)</f>
+        <f t="shared" ref="D18:D21" si="3">($H$5*$H$4^3)/(3*$J$3*$H$2)</f>
         <v>4.7999625002929669</v>
       </c>
       <c r="E18" s="3">
@@ -2869,7 +2871,7 @@
       <c r="F22" s="1"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="E24" s="4">
+      <c r="E24">
         <f>(LN(E20)-LN(E19))/(LN(B20)-LN(B19))</f>
         <v>0.15871517356454326</v>
       </c>

</xml_diff>